<commit_message>
I have added another line, from Russia
</commit_message>
<xml_diff>
--- a/Атрибуты доступные к редактированию.xlsx
+++ b/Атрибуты доступные к редактированию.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Можно редактировать Инициатору АД на статусах «Заявка», «Заявка на согласовании»</t>
   </si>
@@ -894,18 +894,29 @@
   </si>
   <si>
     <t xml:space="preserve">Атрибуты которые вызвали вопросы </t>
+  </si>
+  <si>
+    <t>Также тут всякое текста, траляля, как дела</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -993,18 +1004,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1285,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,6 +1544,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New changes, I am on fire
</commit_message>
<xml_diff>
--- a/Атрибуты доступные к редактированию.xlsx
+++ b/Атрибуты доступные к редактированию.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Можно редактировать Инициатору АД на статусах «Заявка», «Заявка на согласовании»</t>
   </si>
@@ -897,6 +897,9 @@
   </si>
   <si>
     <t>Также тут всякое текста, траляля, как дела</t>
+  </si>
+  <si>
+    <t>And here I am</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,6 +1552,11 @@
         <v>57</v>
       </c>
     </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>